<commit_message>
Updated the describtion of the resistor before the BD139
</commit_message>
<xml_diff>
--- a/3D_Printer_Files/Components.xlsx
+++ b/3D_Printer_Files/Components.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66bda0e3312437e7/02 Arduino/01_Projects/Radiator_fans/3D_Printer_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{6989C354-57FB-4305-B2C3-5D0F3D22BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{812306E4-EA35-4430-AF65-95726FAD943A}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{6989C354-57FB-4305-B2C3-5D0F3D22BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBFA9A5C-F88D-4D50-AD04-4F391A1BB92E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{FDE711AF-7D70-41A4-9CC0-064A34C0C155}"/>
   </bookViews>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+  <si>
+    <t>Implemented</t>
+  </si>
   <si>
     <t>Green is ready to be mounted</t>
   </si>
@@ -67,6 +71,9 @@
     <t>Slave</t>
   </si>
   <si>
+    <t>To be printed</t>
+  </si>
+  <si>
     <t>According to Speedcomfort the air in the room needs to be refreshed once per hour. Their unit moves 30m3/h. So for a room of 8x4x3 = 96 m3. A minimum of 3 speedcomfort units is needed. The unit that I made transfers per fan max 14,5m3. It is not desired that it runs at 100%, but on the other hand the lowest value is 55 a 60% due to the startup voltage needed. The master with extension has 3 fans, assume it runs at 60% with a  airflow of 3x14.5x0.5=21.75 as minimum and 3x14.5=43.5 maximum with noise of the fans.</t>
   </si>
   <si>
@@ -94,10 +101,13 @@
     <t>Kleine kamer</t>
   </si>
   <si>
+    <t>al getekend en past mogelijk ook op de gang</t>
+  </si>
+  <si>
     <t>Master Bedroom</t>
   </si>
   <si>
-    <t>Tessa</t>
+    <t>Tessa. vervallen is naar douche gegaan</t>
   </si>
   <si>
     <t xml:space="preserve">Tessa = ~ 3.5x4x2.2=30.8 m3. Meaning half power 2 units are needed </t>
@@ -200,19 +210,13 @@
   </si>
   <si>
     <t>screw flat head M2x8 om de extension te koppelen</t>
-  </si>
-  <si>
-    <t>To be printed</t>
-  </si>
-  <si>
-    <t>al getekend en past mogelijk ook op de gang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +268,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -308,13 +312,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -626,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690F0E7B-7738-45E7-8CBA-64294AB32761}">
-  <dimension ref="B1:R46"/>
+  <dimension ref="B1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
@@ -647,130 +649,106 @@
     <col min="17" max="17" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3" t="s">
+    <row r="1" spans="2:18">
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18">
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="Q3" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="12" t="s">
+      <c r="J4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="12">
+      <c r="L4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="D5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="10">
         <v>40</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F5" s="10">
         <v>265</v>
       </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12">
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
         <v>3</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J5" s="10">
         <v>3</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="L5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="6" spans="2:18">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="E6">
-        <v>99</v>
-      </c>
-      <c r="F6">
-        <v>84</v>
+      <c r="F6" t="s">
+        <v>17</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
       <c r="B7">
         <v>6</v>
       </c>
@@ -778,57 +756,56 @@
         <v>18</v>
       </c>
       <c r="E7">
+        <v>99</v>
+      </c>
+      <c r="F7">
+        <v>84</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10">
         <v>60</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="10">
         <v>80</v>
       </c>
-      <c r="G7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="G8" s="10">
+        <v>1</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E8">
-        <v>60</v>
-      </c>
-      <c r="F8">
-        <v>168</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>9</v>
-      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
       <c r="D9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>60</v>
@@ -836,251 +813,246 @@
       <c r="F9">
         <v>168</v>
       </c>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="9">
-        <v>2</v>
-      </c>
-      <c r="J9" s="9">
-        <v>2</v>
-      </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10">
+        <v>9</v>
+      </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>60</v>
       </c>
       <c r="F10">
+        <v>168</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="10">
+        <v>2</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11">
+        <v>60</v>
+      </c>
+      <c r="F11">
         <v>84</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1">
         <v>100</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>144</v>
       </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12">
-        <f>SUM(G4:G11)</f>
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ref="H12:J12" si="0">SUM(H4:H11)</f>
-        <v>4</v>
-      </c>
-      <c r="I12">
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <f>SUM(G5:G12)</f>
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:J13" si="0">SUM(H5:H12)</f>
+        <v>5</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="M14" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="R15">
-        <f>SUM(R17:R36)</f>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="M15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16">
+        <f>SUM(R18:R37)</f>
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3" t="s">
+    <row r="17" spans="2:18">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" t="s">
-        <v>29</v>
-      </c>
-      <c r="R16" t="s">
+      <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <f>G$12*C17</f>
-        <v>12</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="M17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="4">
-        <v>21</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17">
-        <v>5</v>
-      </c>
-      <c r="R17">
-        <f>M17*Q17</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
       <c r="B18">
-        <f t="shared" ref="B18:B32" si="1">G$12*C18</f>
-        <v>12</v>
+        <f>G$13*C18</f>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M18" s="4">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="R18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+        <f>M18*Q18</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
       <c r="B19">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" ref="B19:B33" si="1">G$13*C19</f>
+        <v>15</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M19" s="4">
         <v>33</v>
       </c>
-      <c r="M19" s="4">
-        <v>11</v>
-      </c>
       <c r="N19" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="R19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18">
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M20" s="4">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R20">
-        <f t="shared" ref="R20:R21" si="2">M20*Q20</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18">
       <c r="B21">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M21" s="4">
         <v>4</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -1088,356 +1060,371 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R21:R22" si="2">M21*Q21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
       <c r="B22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M22" s="4">
         <v>4</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18">
       <c r="B23">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="4">
         <v>4</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>37</v>
-      </c>
-      <c r="M23" s="4">
-        <v>18</v>
-      </c>
       <c r="N23" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R23">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18">
       <c r="B24">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M24" s="4">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
+      <c r="Q24">
+        <v>4</v>
+      </c>
       <c r="R24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18">
       <c r="B25">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M25" s="4">
         <v>4</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="R25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18">
       <c r="B26">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="M26" s="4">
         <v>4</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="4">
-        <v>11</v>
-      </c>
       <c r="N26" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="R26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18">
       <c r="B27">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M27" s="4">
         <v>11</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="R27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18">
       <c r="B28">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M28" s="4">
         <v>11</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="R28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18">
       <c r="B29">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M29" s="4">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="R29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18">
       <c r="B30">
         <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" s="4">
         <v>4</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>45</v>
-      </c>
-      <c r="M30" s="4">
-        <v>11</v>
-      </c>
       <c r="N30" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18">
       <c r="B31">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M31" s="4">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18">
       <c r="B32">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M32" s="4">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16">
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
       <c r="M33" s="4">
+        <v>33</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="M34" s="4">
         <v>11</v>
       </c>
-      <c r="N33" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="M34" s="4"/>
       <c r="N34" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>21</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="M36" s="4">
-        <v>7</v>
-      </c>
+    <row r="36" spans="2:16">
+      <c r="C36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M36" s="4"/>
       <c r="N36" s="4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="O36" s="4"/>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="2:16">
       <c r="B37">
-        <f t="shared" ref="B37:B46" si="3">I$12*C37</f>
         <v>21</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="M37" s="4">
+        <v>7</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O37" s="4"/>
+    </row>
+    <row r="38" spans="2:16">
       <c r="B38">
+        <f t="shared" ref="B38:B47" si="3">I$13*C38</f>
+        <v>21</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
+      <c r="B39">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16">
+      <c r="B40">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>2</v>
       </c>
-      <c r="D39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
       <c r="D40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16">
       <c r="B41">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1446,10 +1433,10 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16">
       <c r="B42">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1458,10 +1445,10 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
       <c r="B43">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1470,10 +1457,10 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16">
       <c r="B44">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -1482,37 +1469,49 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16">
       <c r="B45">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
       <c r="B46">
         <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16">
+      <c r="B47">
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
-        <v>47</v>
+      <c r="D47" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{61BCAC74-0B40-433E-9725-39439F198569}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{DA9F6C79-A51F-4739-9D45-87A6651A76F2}"/>
+    <hyperlink ref="O3" r:id="rId1" xr:uid="{61BCAC74-0B40-433E-9725-39439F198569}"/>
+    <hyperlink ref="Q3" r:id="rId2" xr:uid="{DA9F6C79-A51F-4739-9D45-87A6651A76F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>